<commit_message>
fix: Adding the missing boolean field of the status of the user or laboratory
</commit_message>
<xml_diff>
--- a/Tabela de Instâncias/instance_tables.xlsx
+++ b/Tabela de Instâncias/instance_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebarbosa\OneDrive - Baymetrics Tecnologia\Documentos\Projetos\Repositorios\SysLab\Tabela de Instâncias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A0142DB6-DB66-4B65-BF1D-94B79561B005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF0151B-2AF5-4622-B54E-EE48063F966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" activeTab="1" xr2:uid="{44B2C8B3-BD36-4029-BB38-8BB839F4ACC4}"/>
+    <workbookView xWindow="2715" yWindow="-13620" windowWidth="24240" windowHeight="13740" xr2:uid="{44B2C8B3-BD36-4029-BB38-8BB839F4ACC4}"/>
   </bookViews>
   <sheets>
     <sheet name="schema_system" sheetId="5" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <definedName name="DadosExternos_1" localSheetId="1" hidden="1">schema_log!$B$3:$G$20</definedName>
     <definedName name="DadosExternos_1" localSheetId="0" hidden="1">schema_system!$B$3:$I$13</definedName>
     <definedName name="DadosExternos_2" localSheetId="1" hidden="1">schema_log!$B$23:$D$26</definedName>
-    <definedName name="DadosExternos_2" localSheetId="0" hidden="1">schema_system!$K$3:$S$10</definedName>
+    <definedName name="DadosExternos_2" localSheetId="0" hidden="1">schema_system!$M$3:$U$10</definedName>
     <definedName name="DadosExternos_3" localSheetId="1" hidden="1">schema_log!$F$23:$H$26</definedName>
     <definedName name="DadosExternos_3" localSheetId="0" hidden="1">schema_system!$I$17:$K$23</definedName>
     <definedName name="DadosExternos_4" localSheetId="1" hidden="1">schema_log!$I$3:$L$5</definedName>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
   <si>
     <t>id</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>log.user_login_logout</t>
+  </si>
+  <si>
+    <t>is_activated</t>
   </si>
 </sst>
 </file>
@@ -982,42 +985,29 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1027,10 +1017,16 @@
     <xf numFmtId="0" fontId="13" fillId="46" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="48" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1076,7 +1072,99 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="38">
+  <dxfs count="46">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC3C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC3C3"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="9" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1089,6 +1177,17 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
           <bgColor theme="9" tint="0.59999389629810485"/>
         </patternFill>
       </fill>
@@ -1102,6 +1201,26 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="8" tint="0.59999389629810485"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFCC99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1118,10 +1237,49 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
+          <bgColor theme="8" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1129,49 +1287,26 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
+          <bgColor theme="6" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFFFCC99"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
       <fill>
         <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="9" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.59999389629810485"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFCC99"/>
+          <bgColor rgb="FF996600"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1213,114 +1348,24 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF996600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yyyy\ hh:mm"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="6" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela 1" pivot="0" count="2" xr9:uid="{B60C7231-DAAE-43D6-83A8-6E31A707EB2E}">
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="45"/>
+      <tableStyleElement type="firstRowStripe" dxfId="44"/>
     </tableStyle>
     <tableStyle name="Estilo de Tabela 2" pivot="0" count="2" xr9:uid="{952573FD-32E3-4E88-B535-8DFABEFF6F49}">
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="firstRowStripe" dxfId="14"/>
+      <tableStyleElement type="headerRow" dxfId="43"/>
+      <tableStyleElement type="firstRowStripe" dxfId="42"/>
     </tableStyle>
-    <tableStyle name="generic" pivot="0" count="3" xr9:uid="{E0A0D11A-3001-4644-BD0A-1E62F00EBC14}">
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
+    <tableStyle name="generic" pivot="0" count="2" xr9:uid="{E0A0D11A-3001-4644-BD0A-1E62F00EBC14}">
+      <tableStyleElement type="headerRow" dxfId="41"/>
+      <tableStyleElement type="firstRowStripe" dxfId="40"/>
     </tableStyle>
   </tableStyles>
   <colors>
     <mruColors>
+      <color rgb="FFFFC3C3"/>
       <color rgb="FFFFCC99"/>
       <color rgb="FF996600"/>
       <color rgb="FF6600CC"/>
@@ -1330,7 +1375,6 @@
       <color rgb="FFCC9900"/>
       <color rgb="FF663300"/>
       <color rgb="FFFF9999"/>
-      <color rgb="FFCCFFCC"/>
     </mruColors>
   </colors>
   <extLst>
@@ -1358,8 +1402,8 @@
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_2" connectionId="7" xr16:uid="{B1A46E61-4503-4E82-B30D-E95A31900005}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="10">
-    <queryTableFields count="9">
+  <queryTableRefresh nextId="11" unboundColumnsRight="1">
+    <queryTableFields count="10">
       <queryTableField id="1" name="id" tableColumnId="1"/>
       <queryTableField id="2" name="enviroment_id" tableColumnId="2"/>
       <queryTableField id="3" name="qtd_computers" tableColumnId="3"/>
@@ -1369,6 +1413,7 @@
       <queryTableField id="7" name="air_conditioner" tableColumnId="7"/>
       <queryTableField id="8" name="opening_time" tableColumnId="8"/>
       <queryTableField id="9" name="closing_time" tableColumnId="9"/>
+      <queryTableField id="10" dataBound="0" tableColumnId="10"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -1376,8 +1421,8 @@
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_1" connectionId="9" xr16:uid="{CC569CC7-55D9-4FA0-9A9B-0914918B6828}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="9">
-    <queryTableFields count="8">
+  <queryTableRefresh nextId="10" unboundColumnsRight="1">
+    <queryTableFields count="9">
       <queryTableField id="1" name="id" tableColumnId="1"/>
       <queryTableField id="2" name="registery" tableColumnId="2"/>
       <queryTableField id="3" name="type" tableColumnId="3"/>
@@ -1386,6 +1431,7 @@
       <queryTableField id="6" name="password" tableColumnId="6"/>
       <queryTableField id="7" name="entry_time" tableColumnId="7"/>
       <queryTableField id="8" name="departure_time" tableColumnId="8"/>
+      <queryTableField id="9" dataBound="0" tableColumnId="9"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
@@ -1479,43 +1525,45 @@
   <autoFilter ref="I17:K23" xr:uid="{53A918CD-5EBA-4EF8-9FD6-87A7A2CD7C3E}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{A6876E42-44EF-4956-AF69-3C2D6B04F05D}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{7A325E24-BE39-48DA-9EE7-B0D3B27379C5}" uniqueName="2" name="user_id" queryTableFieldId="2" dataDxfId="37"/>
-    <tableColumn id="3" xr3:uid="{BE2AB8FB-6C0D-472C-B196-BA1BF6251146}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="36"/>
+    <tableColumn id="2" xr3:uid="{7A325E24-BE39-48DA-9EE7-B0D3B27379C5}" uniqueName="2" name="user_id" queryTableFieldId="2" dataDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{BE2AB8FB-6C0D-472C-B196-BA1BF6251146}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="38"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57C59DB0-9249-446E-B77D-DB2AD692BD9E}" name="system_laboratories" displayName="system_laboratories" ref="K3:S10" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="K3:S10" xr:uid="{57C59DB0-9249-446E-B77D-DB2AD692BD9E}"/>
-  <tableColumns count="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{57C59DB0-9249-446E-B77D-DB2AD692BD9E}" name="system_laboratories" displayName="system_laboratories" ref="M3:V10" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="M3:V10" xr:uid="{57C59DB0-9249-446E-B77D-DB2AD692BD9E}"/>
+  <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CF9F54B0-2B16-4803-B797-3062E9C610A7}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{78188164-6FB0-4347-98E4-08F5EE17E7A6}" uniqueName="2" name="enviroment_id" queryTableFieldId="2" dataDxfId="35"/>
+    <tableColumn id="2" xr3:uid="{78188164-6FB0-4347-98E4-08F5EE17E7A6}" uniqueName="2" name="enviroment_id" queryTableFieldId="2" dataDxfId="37"/>
     <tableColumn id="3" xr3:uid="{504E1429-7582-48F2-9EFB-10FA5FC36F67}" uniqueName="3" name="qtd_computers" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A5BB4F58-0B79-4B51-AA4D-D9A122CAECBA}" uniqueName="4" name="qtd_chairs" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C91A198F-486D-4FF7-8134-3A0EC3966A55}" uniqueName="5" name="television" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{385349E3-86B2-4907-8665-FC59A3BB2ABF}" uniqueName="6" name="fan" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{821EC72B-DABC-4539-87B8-3A65E6E55C50}" uniqueName="7" name="air_conditioner" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{D38230E2-658A-495F-9DFE-3C9960243C45}" uniqueName="8" name="opening_time" queryTableFieldId="8" dataDxfId="34"/>
-    <tableColumn id="9" xr3:uid="{37E81A61-9516-4998-AF1E-4C302EBD35F1}" uniqueName="9" name="closing_time" queryTableFieldId="9" dataDxfId="33"/>
+    <tableColumn id="8" xr3:uid="{D38230E2-658A-495F-9DFE-3C9960243C45}" uniqueName="8" name="opening_time" queryTableFieldId="8" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{37E81A61-9516-4998-AF1E-4C302EBD35F1}" uniqueName="9" name="closing_time" queryTableFieldId="9" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{F34F4038-7D72-46D5-A4A6-38C4C9A0E11D}" uniqueName="10" name="is_activated" queryTableFieldId="10" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5A99A2A-ADE2-467B-BD22-9FEE08578871}" name="system_users" displayName="system_users" ref="B3:I13" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="B3:I13" xr:uid="{B5A99A2A-ADE2-467B-BD22-9FEE08578871}"/>
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B5A99A2A-ADE2-467B-BD22-9FEE08578871}" name="system_users" displayName="system_users" ref="B3:J13" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="B3:J13" xr:uid="{B5A99A2A-ADE2-467B-BD22-9FEE08578871}"/>
+  <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E8957FF5-5CF1-48BE-B563-9D045094127B}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{1EA86638-7101-46C9-AE97-A79DB947852D}" uniqueName="2" name="registery" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{DAAA3AC6-32B6-4B92-848E-82BC6B6135B9}" uniqueName="3" name="type" queryTableFieldId="3" dataDxfId="32"/>
-    <tableColumn id="4" xr3:uid="{6F158A4B-EEB4-4EF1-AA68-EB005873D22D}" uniqueName="4" name="name" queryTableFieldId="4" dataDxfId="31"/>
-    <tableColumn id="5" xr3:uid="{EB6896FB-AF75-4511-9371-9B9F5D8DD646}" uniqueName="5" name="email" queryTableFieldId="5" dataDxfId="30"/>
-    <tableColumn id="6" xr3:uid="{882919FE-1CCF-46B5-9E1D-EFE6F9E221F0}" uniqueName="6" name="password" queryTableFieldId="6" dataDxfId="29"/>
-    <tableColumn id="7" xr3:uid="{F197965F-C0E5-4D0E-A0C8-38DCFD90D9AC}" uniqueName="7" name="entry_time" queryTableFieldId="7" dataDxfId="28"/>
-    <tableColumn id="8" xr3:uid="{BCD822DB-C994-4301-8B4B-AB18371426B6}" uniqueName="8" name="departure_time" queryTableFieldId="8" dataDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{DAAA3AC6-32B6-4B92-848E-82BC6B6135B9}" uniqueName="3" name="type" queryTableFieldId="3" dataDxfId="34"/>
+    <tableColumn id="4" xr3:uid="{6F158A4B-EEB4-4EF1-AA68-EB005873D22D}" uniqueName="4" name="name" queryTableFieldId="4" dataDxfId="33"/>
+    <tableColumn id="5" xr3:uid="{EB6896FB-AF75-4511-9371-9B9F5D8DD646}" uniqueName="5" name="email" queryTableFieldId="5" dataDxfId="32"/>
+    <tableColumn id="6" xr3:uid="{882919FE-1CCF-46B5-9E1D-EFE6F9E221F0}" uniqueName="6" name="password" queryTableFieldId="6" dataDxfId="31"/>
+    <tableColumn id="7" xr3:uid="{F197965F-C0E5-4D0E-A0C8-38DCFD90D9AC}" uniqueName="7" name="entry_time" queryTableFieldId="7" dataDxfId="30"/>
+    <tableColumn id="8" xr3:uid="{BCD822DB-C994-4301-8B4B-AB18371426B6}" uniqueName="8" name="departure_time" queryTableFieldId="8" dataDxfId="29"/>
+    <tableColumn id="9" xr3:uid="{03BB6B96-6738-4D16-8BB1-5856A5FADCCB}" uniqueName="9" name="is_activated" queryTableFieldId="9" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1526,10 +1574,10 @@
   <autoFilter ref="B3:G20" xr:uid="{CCE5E823-FA9A-46C1-AEE5-A1F4D26E97D2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6DD82B72-16FA-4522-9E0D-76CD3A296400}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{DB60987B-C92B-4400-9315-A645299F690D}" uniqueName="2" name="type" queryTableFieldId="2" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{155B98F5-19F9-4323-8010-D88AEC622683}" uniqueName="3" name="create_time" queryTableFieldId="3" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{5DD35A2A-535E-4AC9-AD6E-9C57089C59EA}" uniqueName="4" name="desc" queryTableFieldId="4" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{6799B699-560A-4E69-B293-35BFF90C76F4}" uniqueName="5" name="children_logs" queryTableFieldId="5" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{DB60987B-C92B-4400-9315-A645299F690D}" uniqueName="2" name="type" queryTableFieldId="2" dataDxfId="28"/>
+    <tableColumn id="3" xr3:uid="{155B98F5-19F9-4323-8010-D88AEC622683}" uniqueName="3" name="create_time" queryTableFieldId="3" dataDxfId="27"/>
+    <tableColumn id="4" xr3:uid="{5DD35A2A-535E-4AC9-AD6E-9C57089C59EA}" uniqueName="4" name="desc" queryTableFieldId="4" dataDxfId="26"/>
+    <tableColumn id="5" xr3:uid="{6799B699-560A-4E69-B293-35BFF90C76F4}" uniqueName="5" name="children_logs" queryTableFieldId="5" dataDxfId="25"/>
     <tableColumn id="6" xr3:uid="{C9D06D86-02D2-4AA9-B04D-10B8753863E4}" uniqueName="6" name="responsible_user" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="generic" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1541,8 +1589,8 @@
   <autoFilter ref="B23:D26" xr:uid="{D29CA22D-8193-455B-B30F-40F9B9CD21C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D8614071-7ED6-4F35-A407-2B26683179ED}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{5C87E7F9-259D-4C99-86D4-1187DB56973D}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{22F785A3-4A76-4040-B33C-F9F005C7667B}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{5C87E7F9-259D-4C99-86D4-1187DB56973D}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{22F785A3-4A76-4040-B33C-F9F005C7667B}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de Tabela 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1553,8 +1601,8 @@
   <autoFilter ref="F23:H26" xr:uid="{553991DF-4562-4DC9-B4D7-CACE9EC4EF9C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4110A2A1-680D-49EE-A555-BAB59838AABD}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{7C89E2E5-6182-4820-BB2D-018B26C39F30}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{5B1AA004-F95E-4671-98A9-F506460937ED}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{7C89E2E5-6182-4820-BB2D-018B26C39F30}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="22"/>
+    <tableColumn id="3" xr3:uid="{5B1AA004-F95E-4671-98A9-F506460937ED}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de Tabela 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1565,9 +1613,9 @@
   <autoFilter ref="I3:L5" xr:uid="{2E646A49-017A-408A-9130-31769D85C05F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3D491E2-3254-434B-A6D1-2BD498E19A2D}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{E42B4EE0-3A8F-47F8-A9FB-225337B26D45}" uniqueName="5" name="laboratory_list" queryTableFieldId="5" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{C3A4A2CF-8E80-435C-84B2-536EC81F67C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{10E92AEF-AA7D-4B7E-A6B2-9C4DFAD41D6F}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{E42B4EE0-3A8F-47F8-A9FB-225337B26D45}" uniqueName="5" name="laboratory_list" queryTableFieldId="5" dataDxfId="20"/>
+    <tableColumn id="2" xr3:uid="{C3A4A2CF-8E80-435C-84B2-536EC81F67C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="4" xr3:uid="{10E92AEF-AA7D-4B7E-A6B2-9C4DFAD41D6F}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1578,10 +1626,10 @@
   <autoFilter ref="I8:M13" xr:uid="{852D41C6-0DEC-4824-B44E-DEA0AE43A72A}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{C910F50F-3F72-4039-8AE2-5D47546A804C}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{A042CA4C-1840-492F-9D9B-29679C65384A}" uniqueName="5" name="status" queryTableFieldId="5" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{3062A848-4CA3-4E74-B625-1F9A900401EC}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{09894099-35FD-4465-A043-0F0FA29B9B44}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{2B76CF40-5649-4C92-840F-F3F52BA8BB01}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A042CA4C-1840-492F-9D9B-29679C65384A}" uniqueName="5" name="status" queryTableFieldId="5" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{3062A848-4CA3-4E74-B625-1F9A900401EC}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{09894099-35FD-4465-A043-0F0FA29B9B44}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{2B76CF40-5649-4C92-840F-F3F52BA8BB01}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1592,10 +1640,10 @@
   <autoFilter ref="I16:M20" xr:uid="{FA7BCB58-3694-4DE3-9863-1776FE39B818}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{62BA4DE1-B2BB-4F72-BE20-471A357DC53B}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="4" xr3:uid="{F1B0659D-A210-4A2D-B394-E87FB9BC2043}" uniqueName="4" name="operation_type" queryTableFieldId="4" dataDxfId="22"/>
-    <tableColumn id="5" xr3:uid="{FC65033A-F10C-4B71-852E-10A386498392}" uniqueName="5" name="session_key" queryTableFieldId="5" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{D4E4A59B-332D-44FC-80DC-6D187F5821C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{4619D07E-E77D-4FAC-9DD2-906F21BF18C8}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{F1B0659D-A210-4A2D-B394-E87FB9BC2043}" uniqueName="4" name="operation_type" queryTableFieldId="4" dataDxfId="13"/>
+    <tableColumn id="5" xr3:uid="{FC65033A-F10C-4B71-852E-10A386498392}" uniqueName="5" name="session_key" queryTableFieldId="5" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{D4E4A59B-332D-44FC-80DC-6D187F5821C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{4619D07E-E77D-4FAC-9DD2-906F21BF18C8}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1918,10 +1966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC27D49-7F91-4D20-84B4-93EC05C08DA3}">
-  <dimension ref="B2:S23"/>
+  <dimension ref="B2:V23"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="R31" sqref="R31"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="V11" sqref="V11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1934,7 +1982,7 @@
     <col min="7" max="7" width="18" customWidth="1"/>
     <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
@@ -1944,32 +1992,35 @@
     <col min="17" max="17" width="17" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B2" s="9" t="s">
+    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="B2" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="8"/>
-      <c r="K2" s="11" t="s">
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="M2" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
-      <c r="S2" s="10"/>
-    </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="15"/>
+      <c r="Q2" s="15"/>
+      <c r="R2" s="15"/>
+      <c r="S2" s="15"/>
+      <c r="T2" s="15"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="15"/>
+    </row>
+    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1994,498 +2045,555 @@
       <c r="I3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
+      <c r="J3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M3" t="s">
         <v>0</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="O3" t="s">
         <v>43</v>
       </c>
-      <c r="N3" t="s">
+      <c r="P3" t="s">
         <v>44</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>45</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="S3" t="s">
         <v>47</v>
       </c>
-      <c r="R3" t="s">
+      <c r="T3" t="s">
         <v>48</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4">
         <v>1001</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="G4" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>0.75</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-      <c r="L4" s="1" t="s">
+      <c r="J4" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
         <v>50</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>30</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>30</v>
       </c>
-      <c r="O4" t="b">
-        <v>1</v>
-      </c>
-      <c r="P4" t="b">
-        <v>1</v>
-      </c>
       <c r="Q4" t="b">
         <v>1</v>
       </c>
-      <c r="R4" s="2">
+      <c r="R4" t="b">
+        <v>1</v>
+      </c>
+      <c r="S4" t="b">
+        <v>1</v>
+      </c>
+      <c r="T4" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="S4" s="2">
+      <c r="U4" s="1">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V4" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
       <c r="C5">
         <v>2010</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="G5" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>0.3125</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>0.72916666666666663</v>
       </c>
-      <c r="K5">
+      <c r="J5" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M5">
         <v>2</v>
       </c>
-      <c r="L5" s="1" t="s">
+      <c r="N5" t="s">
         <v>51</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>28</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>30</v>
       </c>
-      <c r="O5" t="b">
+      <c r="Q5" t="b">
         <v>0</v>
       </c>
-      <c r="P5" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q5" t="b">
-        <v>1</v>
-      </c>
-      <c r="R5" s="2">
+      <c r="R5" t="b">
+        <v>1</v>
+      </c>
+      <c r="S5" t="b">
+        <v>1</v>
+      </c>
+      <c r="T5" s="1">
         <v>0.3125</v>
       </c>
-      <c r="S5" s="2">
+      <c r="U5" s="1">
         <v>0.75</v>
       </c>
-    </row>
-    <row r="6" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V5" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>3</v>
       </c>
       <c r="C6">
         <v>2011</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>16</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="G6" t="s">
         <v>19</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>0.91666666666666663</v>
       </c>
-      <c r="K6">
+      <c r="J6" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M6">
         <v>3</v>
       </c>
-      <c r="L6" s="1" t="s">
+      <c r="N6" t="s">
         <v>52</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>40</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>40</v>
       </c>
-      <c r="O6" t="b">
-        <v>1</v>
-      </c>
-      <c r="P6" t="b">
+      <c r="Q6" t="b">
+        <v>1</v>
+      </c>
+      <c r="R6" t="b">
         <v>0</v>
       </c>
-      <c r="Q6" t="b">
-        <v>1</v>
-      </c>
-      <c r="R6" s="2">
+      <c r="S6" t="b">
+        <v>1</v>
+      </c>
+      <c r="T6" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="S6" s="2">
+      <c r="U6" s="1">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V6" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>4</v>
       </c>
       <c r="C7">
         <v>2012</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
         <v>20</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" t="s">
         <v>23</v>
       </c>
-      <c r="H7" s="2">
+      <c r="H7" s="1">
         <v>0.34375</v>
       </c>
-      <c r="I7" s="2">
+      <c r="I7" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="K7">
+      <c r="J7" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M7">
         <v>4</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="N7" t="s">
         <v>53</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>23</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>25</v>
-      </c>
-      <c r="O7" t="b">
-        <v>0</v>
-      </c>
-      <c r="P7" t="b">
-        <v>1</v>
       </c>
       <c r="Q7" t="b">
         <v>0</v>
       </c>
-      <c r="R7" s="2">
+      <c r="R7" t="b">
+        <v>1</v>
+      </c>
+      <c r="S7" t="b">
+        <v>0</v>
+      </c>
+      <c r="T7" s="1">
         <v>0.54166666666666663</v>
       </c>
-      <c r="S7" s="2">
+      <c r="U7" s="1">
         <v>0.875</v>
       </c>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V7" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
       <c r="C8">
         <v>2013</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" t="s">
         <v>26</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="1">
         <v>0.5</v>
       </c>
-      <c r="I8" s="2">
+      <c r="I8" s="1">
         <v>0.875</v>
       </c>
-      <c r="K8">
+      <c r="J8" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M8">
         <v>5</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N8" t="s">
         <v>54</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>36</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>35</v>
       </c>
-      <c r="O8" t="b">
-        <v>1</v>
-      </c>
-      <c r="P8" t="b">
-        <v>1</v>
-      </c>
       <c r="Q8" t="b">
         <v>1</v>
       </c>
-      <c r="R8" s="2">
+      <c r="R8" t="b">
+        <v>1</v>
+      </c>
+      <c r="S8" t="b">
+        <v>1</v>
+      </c>
+      <c r="T8" s="1">
         <v>0.3125</v>
       </c>
-      <c r="S8" s="2">
+      <c r="U8" s="1">
         <v>0.91666666666666663</v>
       </c>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V8" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>6</v>
       </c>
       <c r="C9">
         <v>2014</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
         <v>16</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>27</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>0.32291666666666669</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>0.73958333333333337</v>
       </c>
-      <c r="K9">
+      <c r="J9" s="22" t="b">
+        <v>1</v>
+      </c>
+      <c r="M9">
         <v>6</v>
       </c>
-      <c r="L9" s="1" t="s">
+      <c r="N9" t="s">
         <v>55</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>20</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>22</v>
-      </c>
-      <c r="O9" t="b">
-        <v>0</v>
-      </c>
-      <c r="P9" t="b">
-        <v>1</v>
       </c>
       <c r="Q9" t="b">
         <v>0</v>
       </c>
-      <c r="R9" s="2">
+      <c r="R9" t="b">
+        <v>1</v>
+      </c>
+      <c r="S9" t="b">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
         <v>0.58333333333333337</v>
       </c>
-      <c r="S9" s="2">
+      <c r="U9" s="1">
         <v>0.83333333333333337</v>
       </c>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V9" s="1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>7</v>
       </c>
       <c r="C10">
         <v>2015</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>30</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="1" t="s">
+      <c r="G10" t="s">
         <v>32</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>0.75</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>0.9375</v>
       </c>
-      <c r="K10">
+      <c r="J10" s="22" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10">
         <v>7</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="N10" t="s">
         <v>56</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>38</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>40</v>
       </c>
-      <c r="O10" t="b">
-        <v>1</v>
-      </c>
-      <c r="P10" t="b">
+      <c r="Q10" t="b">
+        <v>1</v>
+      </c>
+      <c r="R10" t="b">
         <v>0</v>
       </c>
-      <c r="Q10" t="b">
-        <v>1</v>
-      </c>
-      <c r="R10" s="2">
+      <c r="S10" t="b">
+        <v>1</v>
+      </c>
+      <c r="T10" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="S10" s="2">
+      <c r="U10" s="1">
         <v>0.89583333333333337</v>
       </c>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="V10" s="1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>8</v>
       </c>
       <c r="C11">
         <v>2016</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
         <v>20</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>33</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G11" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>0.75694444444444442</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>0.94444444444444442</v>
       </c>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J11" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>9</v>
       </c>
       <c r="C12">
         <v>2017</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>37</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>0.5625</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>0.92708333333333337</v>
       </c>
-    </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.25">
+      <c r="J12" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>10</v>
       </c>
       <c r="C13">
         <v>2018</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" t="s">
         <v>12</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" t="s">
         <v>41</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>0.33333333333333331</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>0.70833333333333337</v>
       </c>
-    </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="I16" s="7" t="s">
+      <c r="J13" s="22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="I16" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="7"/>
-      <c r="K16" s="7"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
     </row>
     <row r="17" spans="9:11" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="4" t="s">
+      <c r="J17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="5" t="s">
+      <c r="K17" s="4" t="s">
         <v>58</v>
       </c>
     </row>
@@ -2493,10 +2601,10 @@
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18" s="2">
         <v>2</v>
       </c>
-      <c r="K18" s="6">
+      <c r="K18" s="5">
         <v>1</v>
       </c>
     </row>
@@ -2504,10 +2612,10 @@
       <c r="I19">
         <v>2</v>
       </c>
-      <c r="J19" s="3">
+      <c r="J19" s="2">
         <v>3</v>
       </c>
-      <c r="K19" s="6">
+      <c r="K19" s="5">
         <v>3</v>
       </c>
     </row>
@@ -2515,10 +2623,10 @@
       <c r="I20">
         <v>3</v>
       </c>
-      <c r="J20" s="3">
+      <c r="J20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K20" s="5">
         <v>2</v>
       </c>
     </row>
@@ -2526,10 +2634,10 @@
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21" s="3">
+      <c r="J21" s="2">
         <v>6</v>
       </c>
-      <c r="K21" s="6">
+      <c r="K21" s="5">
         <v>3</v>
       </c>
     </row>
@@ -2537,10 +2645,10 @@
       <c r="I22">
         <v>5</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J22" s="2">
         <v>9</v>
       </c>
-      <c r="K22" s="6">
+      <c r="K22" s="5">
         <v>5</v>
       </c>
     </row>
@@ -2548,24 +2656,32 @@
       <c r="I23">
         <v>6</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J23" s="2">
         <v>10</v>
       </c>
-      <c r="K23" s="6">
+      <c r="K23" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="I16:K16"/>
-    <mergeCell ref="B2:I2"/>
-    <mergeCell ref="K2:S2"/>
+    <mergeCell ref="B2:J2"/>
+    <mergeCell ref="M2:V2"/>
   </mergeCells>
-  <conditionalFormatting sqref="O4:Q10">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="equal">
+  <conditionalFormatting sqref="J4:J13">
+    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q4:V10">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2582,7 +2698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66D9B545-4BF9-4371-A554-13F6FC1D79B0}">
   <dimension ref="B2:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -2603,20 +2719,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="I2" s="15" t="s">
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="I2" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="15"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
     </row>
     <row r="3" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -2643,10 +2759,10 @@
       <c r="J3" t="s">
         <v>93</v>
       </c>
-      <c r="K3" s="17" t="s">
+      <c r="K3" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2654,16 +2770,16 @@
       <c r="B4">
         <v>1</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" t="s">
         <v>66</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="6">
         <v>45820.60428240741</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" t="s">
         <v>67</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" t="s">
         <v>68</v>
       </c>
       <c r="G4">
@@ -2672,13 +2788,13 @@
       <c r="I4">
         <v>1</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" t="s">
         <v>94</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="8">
         <v>13</v>
       </c>
-      <c r="L4" s="25">
+      <c r="L4" s="12">
         <v>3</v>
       </c>
     </row>
@@ -2686,16 +2802,16 @@
       <c r="B5">
         <v>2</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="6">
         <v>45820.605150462965</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="E5" t="s">
         <v>70</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" t="s">
         <v>71</v>
       </c>
       <c r="G5">
@@ -2704,13 +2820,13 @@
       <c r="I5">
         <v>2</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" t="s">
         <v>95</v>
       </c>
-      <c r="K5" s="18">
+      <c r="K5" s="8">
         <v>14</v>
       </c>
-      <c r="L5" s="25">
+      <c r="L5" s="12">
         <v>6</v>
       </c>
     </row>
@@ -2718,16 +2834,16 @@
       <c r="B6">
         <v>3</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="6">
         <v>45820.605613425927</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="E6" t="s">
         <v>73</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="F6" t="s">
         <v>74</v>
       </c>
       <c r="G6">
@@ -2738,43 +2854,43 @@
       <c r="B7">
         <v>4</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="6">
         <v>45820.606423611112</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="E7" t="s">
         <v>75</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" t="s">
         <v>76</v>
       </c>
       <c r="G7">
         <v>1</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="J7" s="13"/>
-      <c r="K7" s="13"/>
-      <c r="L7" s="13"/>
-      <c r="M7" s="13"/>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+      <c r="L7" s="20"/>
+      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>5</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" t="s">
         <v>69</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="6">
         <v>45820.606944444444</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" t="s">
         <v>77</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" t="s">
         <v>78</v>
       </c>
       <c r="G8">
@@ -2786,13 +2902,13 @@
       <c r="J8" t="s">
         <v>96</v>
       </c>
-      <c r="K8" s="17" t="s">
+      <c r="K8" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="23" t="s">
+      <c r="L8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2800,16 +2916,16 @@
       <c r="B9">
         <v>6</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="6">
         <v>45820.608217592591</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="E9" t="s">
         <v>73</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="F9" t="s">
         <v>79</v>
       </c>
       <c r="G9">
@@ -2818,16 +2934,16 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="J9" t="s">
         <v>97</v>
       </c>
-      <c r="K9" s="18">
+      <c r="K9" s="8">
         <v>10</v>
       </c>
-      <c r="L9" s="24">
-        <v>1</v>
-      </c>
-      <c r="M9" s="25">
+      <c r="L9" s="11">
+        <v>1</v>
+      </c>
+      <c r="M9" s="12">
         <v>2</v>
       </c>
     </row>
@@ -2835,16 +2951,16 @@
       <c r="B10">
         <v>7</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" t="s">
         <v>80</v>
       </c>
-      <c r="D10" s="12">
+      <c r="D10" s="6">
         <v>45820.608449074076</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="E10" t="s">
         <v>73</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="F10" t="s">
         <v>81</v>
       </c>
       <c r="G10">
@@ -2853,16 +2969,16 @@
       <c r="I10">
         <v>2</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="J10" t="s">
         <v>97</v>
       </c>
-      <c r="K10" s="18">
+      <c r="K10" s="8">
         <v>11</v>
       </c>
-      <c r="L10" s="24">
+      <c r="L10" s="11">
         <v>3</v>
       </c>
-      <c r="M10" s="25">
+      <c r="M10" s="12">
         <v>3</v>
       </c>
     </row>
@@ -2870,16 +2986,16 @@
       <c r="B11">
         <v>8</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" t="s">
         <v>80</v>
       </c>
-      <c r="D11" s="12">
+      <c r="D11" s="6">
         <v>45820.609282407408</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="E11" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="F11" t="s">
         <v>82</v>
       </c>
       <c r="G11">
@@ -2888,16 +3004,16 @@
       <c r="I11">
         <v>3</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="J11" t="s">
         <v>98</v>
       </c>
-      <c r="K11" s="18">
+      <c r="K11" s="8">
         <v>12</v>
       </c>
-      <c r="L11" s="24">
-        <v>1</v>
-      </c>
-      <c r="M11" s="25">
+      <c r="L11" s="11">
+        <v>1</v>
+      </c>
+      <c r="M11" s="12">
         <v>2</v>
       </c>
     </row>
@@ -2905,16 +3021,16 @@
       <c r="B12">
         <v>9</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" t="s">
         <v>80</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="6">
         <v>45820.609733796293</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" t="s">
         <v>73</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" t="s">
         <v>83</v>
       </c>
       <c r="G12">
@@ -2923,16 +3039,16 @@
       <c r="I12">
         <v>4</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" t="s">
         <v>98</v>
       </c>
-      <c r="K12" s="18">
+      <c r="K12" s="8">
         <v>16</v>
       </c>
-      <c r="L12" s="24">
+      <c r="L12" s="11">
         <v>4</v>
       </c>
-      <c r="M12" s="25">
+      <c r="M12" s="12">
         <v>10</v>
       </c>
     </row>
@@ -2940,16 +3056,16 @@
       <c r="B13">
         <v>10</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13" s="6">
         <v>45820.610625000001</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" t="s">
         <v>84</v>
       </c>
       <c r="G13">
@@ -2958,16 +3074,16 @@
       <c r="I13">
         <v>5</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" t="s">
         <v>97</v>
       </c>
-      <c r="K13" s="18">
+      <c r="K13" s="8">
         <v>17</v>
       </c>
-      <c r="L13" s="24">
-        <v>1</v>
-      </c>
-      <c r="M13" s="25">
+      <c r="L13" s="11">
+        <v>1</v>
+      </c>
+      <c r="M13" s="12">
         <v>10</v>
       </c>
     </row>
@@ -2975,16 +3091,16 @@
       <c r="B14">
         <v>11</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="12">
+      <c r="D14" s="6">
         <v>45820.611631944441</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" t="s">
         <v>73</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" t="s">
         <v>85</v>
       </c>
       <c r="G14">
@@ -2995,43 +3111,43 @@
       <c r="B15">
         <v>12</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" t="s">
         <v>80</v>
       </c>
-      <c r="D15" s="12">
+      <c r="D15" s="6">
         <v>45820.612442129626</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="E15" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="F15" t="s">
         <v>86</v>
       </c>
       <c r="G15">
         <v>1</v>
       </c>
-      <c r="I15" s="16" t="s">
+      <c r="I15" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
-      <c r="L15" s="16"/>
-      <c r="M15" s="16"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>13</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" t="s">
         <v>80</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16" s="6">
         <v>45820.612881944442</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" t="s">
         <v>73</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" t="s">
         <v>87</v>
       </c>
       <c r="G16">
@@ -3046,10 +3162,10 @@
       <c r="K16" t="s">
         <v>100</v>
       </c>
-      <c r="L16" s="17" t="s">
+      <c r="L16" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M16" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -3057,16 +3173,16 @@
       <c r="B17">
         <v>14</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" t="s">
         <v>80</v>
       </c>
-      <c r="D17" s="12">
+      <c r="D17" s="6">
         <v>45820.613298611112</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" t="s">
         <v>73</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" t="s">
         <v>88</v>
       </c>
       <c r="G17">
@@ -3075,16 +3191,16 @@
       <c r="I17">
         <v>1</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" t="s">
         <v>101</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" t="s">
         <v>102</v>
       </c>
-      <c r="L17" s="18">
+      <c r="L17" s="8">
         <v>7</v>
       </c>
-      <c r="M17" s="25">
+      <c r="M17" s="12">
         <v>3</v>
       </c>
     </row>
@@ -3092,16 +3208,16 @@
       <c r="B18">
         <v>15</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="C18" t="s">
         <v>80</v>
       </c>
-      <c r="D18" s="12">
+      <c r="D18" s="6">
         <v>45820.613888888889</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="E18" t="s">
         <v>73</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" t="s">
         <v>89</v>
       </c>
       <c r="G18">
@@ -3110,16 +3226,16 @@
       <c r="I18">
         <v>2</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="J18" t="s">
         <v>101</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" t="s">
         <v>103</v>
       </c>
-      <c r="L18" s="18">
+      <c r="L18" s="8">
         <v>8</v>
       </c>
-      <c r="M18" s="25">
+      <c r="M18" s="12">
         <v>4</v>
       </c>
     </row>
@@ -3127,16 +3243,16 @@
       <c r="B19">
         <v>16</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" t="s">
         <v>80</v>
       </c>
-      <c r="D19" s="12">
+      <c r="D19" s="6">
         <v>45826.384722222225</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" t="s">
         <v>73</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" t="s">
         <v>90</v>
       </c>
       <c r="G19">
@@ -3145,16 +3261,16 @@
       <c r="I19">
         <v>3</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" t="s">
         <v>104</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" t="s">
         <v>102</v>
       </c>
-      <c r="L19" s="18">
+      <c r="L19" s="8">
         <v>9</v>
       </c>
-      <c r="M19" s="25">
+      <c r="M19" s="12">
         <v>3</v>
       </c>
     </row>
@@ -3162,16 +3278,16 @@
       <c r="B20">
         <v>17</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" t="s">
         <v>80</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="6">
         <v>45826.384780092594</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" t="s">
         <v>73</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" t="s">
         <v>91</v>
       </c>
       <c r="G20">
@@ -3180,48 +3296,48 @@
       <c r="I20">
         <v>4</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" t="s">
         <v>101</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" t="s">
         <v>105</v>
       </c>
-      <c r="L20" s="18">
+      <c r="L20" s="8">
         <v>15</v>
       </c>
-      <c r="M20" s="25">
+      <c r="M20" s="12">
         <v>7</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="17" t="s">
         <v>107</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="F22" s="21" t="s">
+      <c r="C22" s="17"/>
+      <c r="D22" s="17"/>
+      <c r="F22" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="G22" s="21"/>
-      <c r="H22" s="21"/>
+      <c r="G22" s="18"/>
+      <c r="H22" s="18"/>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>0</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="D23" s="22" t="s">
+      <c r="D23" s="9" t="s">
         <v>57</v>
       </c>
       <c r="F23" t="s">
         <v>0</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="H23" s="23" t="s">
+      <c r="H23" s="10" t="s">
         <v>58</v>
       </c>
     </row>
@@ -3229,19 +3345,19 @@
       <c r="B24">
         <v>1</v>
       </c>
-      <c r="C24" s="18">
-        <v>1</v>
-      </c>
-      <c r="D24" s="25">
+      <c r="C24" s="8">
+        <v>1</v>
+      </c>
+      <c r="D24" s="12">
         <v>4</v>
       </c>
       <c r="F24">
         <v>1</v>
       </c>
-      <c r="G24" s="18">
+      <c r="G24" s="8">
         <v>4</v>
       </c>
-      <c r="H24" s="24">
+      <c r="H24" s="11">
         <v>7</v>
       </c>
     </row>
@@ -3249,19 +3365,19 @@
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" s="18">
+      <c r="C25" s="8">
         <v>2</v>
       </c>
-      <c r="D25" s="25">
+      <c r="D25" s="12">
         <v>2</v>
       </c>
       <c r="F25">
         <v>2</v>
       </c>
-      <c r="G25" s="18">
+      <c r="G25" s="8">
         <v>5</v>
       </c>
-      <c r="H25" s="24">
+      <c r="H25" s="11">
         <v>4</v>
       </c>
     </row>
@@ -3269,19 +3385,19 @@
       <c r="B26">
         <v>3</v>
       </c>
-      <c r="C26" s="18">
+      <c r="C26" s="8">
         <v>3</v>
       </c>
-      <c r="D26" s="25">
+      <c r="D26" s="12">
         <v>8</v>
       </c>
       <c r="F26">
         <v>3</v>
       </c>
-      <c r="G26" s="18">
+      <c r="G26" s="8">
         <v>6</v>
       </c>
-      <c r="H26" s="24">
+      <c r="H26" s="11">
         <v>6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix: Moving and transpassing the status fiels from the log table about the assosiation between the users and laboratories to the system's table responsable to assosiate them as a boolean field
</commit_message>
<xml_diff>
--- a/Tabela de Instâncias/instance_tables.xlsx
+++ b/Tabela de Instâncias/instance_tables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ebarbosa\OneDrive - Baymetrics Tecnologia\Documentos\Projetos\Repositorios\SysLab\Tabela de Instâncias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AF0151B-2AF5-4622-B54E-EE48063F966A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3D6925-5041-49B5-9CD8-3D12E44CA145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2715" yWindow="-13620" windowWidth="24240" windowHeight="13740" xr2:uid="{44B2C8B3-BD36-4029-BB38-8BB839F4ACC4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{44B2C8B3-BD36-4029-BB38-8BB839F4ACC4}"/>
   </bookViews>
   <sheets>
     <sheet name="schema_system" sheetId="5" r:id="rId1"/>
@@ -22,9 +22,9 @@
     <definedName name="DadosExternos_2" localSheetId="1" hidden="1">schema_log!$B$23:$D$26</definedName>
     <definedName name="DadosExternos_2" localSheetId="0" hidden="1">schema_system!$M$3:$U$10</definedName>
     <definedName name="DadosExternos_3" localSheetId="1" hidden="1">schema_log!$F$23:$H$26</definedName>
-    <definedName name="DadosExternos_3" localSheetId="0" hidden="1">schema_system!$I$17:$K$23</definedName>
+    <definedName name="DadosExternos_3" localSheetId="0" hidden="1">schema_system!$I$17:$L$23</definedName>
     <definedName name="DadosExternos_4" localSheetId="1" hidden="1">schema_log!$I$3:$L$5</definedName>
-    <definedName name="DadosExternos_5" localSheetId="1" hidden="1">schema_log!$I$8:$M$13</definedName>
+    <definedName name="DadosExternos_5" localSheetId="1" hidden="1">schema_log!$I$8:$L$13</definedName>
     <definedName name="DadosExternos_6" localSheetId="1" hidden="1">schema_log!$I$16:$M$20</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="111">
   <si>
     <t>id</t>
   </si>
@@ -354,15 +354,6 @@
     <t>[{"id": 3, "enviroment_id": "103AC"}]</t>
   </si>
   <si>
-    <t>status</t>
-  </si>
-  <si>
-    <t>granted</t>
-  </si>
-  <si>
-    <t>revoked</t>
-  </si>
-  <si>
     <t>operation_type</t>
   </si>
   <si>
@@ -403,6 +394,9 @@
   </si>
   <si>
     <t>is_activated</t>
+  </si>
+  <si>
+    <t>allowed</t>
   </si>
 </sst>
 </file>
@@ -985,7 +979,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -1026,7 +1020,6 @@
     <xf numFmtId="0" fontId="13" fillId="42" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Ênfase1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1072,7 +1065,35 @@
     <cellStyle name="Título 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="46">
+  <dxfs count="43">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCCFFCC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF9999"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1086,54 +1107,6 @@
           <bgColor rgb="FFFFC3C3"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCCFFCC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF9999"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC3C3"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <fill>
@@ -1182,9 +1155,6 @@
       </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <fgColor indexed="64"/>
@@ -1249,6 +1219,9 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
@@ -1265,6 +1238,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
@@ -1351,16 +1327,16 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Estilo de Tabela 1" pivot="0" count="2" xr9:uid="{B60C7231-DAAE-43D6-83A8-6E31A707EB2E}">
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
+      <tableStyleElement type="headerRow" dxfId="42"/>
+      <tableStyleElement type="firstRowStripe" dxfId="41"/>
     </tableStyle>
     <tableStyle name="Estilo de Tabela 2" pivot="0" count="2" xr9:uid="{952573FD-32E3-4E88-B535-8DFABEFF6F49}">
-      <tableStyleElement type="headerRow" dxfId="43"/>
-      <tableStyleElement type="firstRowStripe" dxfId="42"/>
+      <tableStyleElement type="headerRow" dxfId="40"/>
+      <tableStyleElement type="firstRowStripe" dxfId="39"/>
     </tableStyle>
     <tableStyle name="generic" pivot="0" count="2" xr9:uid="{E0A0D11A-3001-4644-BD0A-1E62F00EBC14}">
-      <tableStyleElement type="headerRow" dxfId="41"/>
-      <tableStyleElement type="firstRowStripe" dxfId="40"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="firstRowStripe" dxfId="37"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1390,9 +1366,10 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_3" connectionId="8" xr16:uid="{16E5F4C1-9D26-4BEC-8989-AB3068890AF1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="4">
-    <queryTableFields count="3">
+  <queryTableRefresh nextId="5">
+    <queryTableFields count="4">
       <queryTableField id="1" name="id" tableColumnId="1"/>
+      <queryTableField id="4" dataBound="0" tableColumnId="4"/>
       <queryTableField id="2" name="user_id" tableColumnId="2"/>
       <queryTableField id="3" name="laboratory_id" tableColumnId="3"/>
     </queryTableFields>
@@ -1495,13 +1472,15 @@
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="DadosExternos_5" connectionId="1" xr16:uid="{6FF843B9-CBD9-4101-BE65-2CD412C16154}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="7">
-    <queryTableFields count="5">
+    <queryTableFields count="4">
       <queryTableField id="1" name="id" tableColumnId="1"/>
-      <queryTableField id="5" name="status" tableColumnId="5"/>
       <queryTableField id="2" name="generic_id" tableColumnId="2"/>
       <queryTableField id="3" name="laboratory_id" tableColumnId="3"/>
       <queryTableField id="4" name="user_id" tableColumnId="4"/>
     </queryTableFields>
+    <queryTableDeletedFields count="1">
+      <deletedField name="status"/>
+    </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
 </file>
@@ -1521,12 +1500,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53A918CD-5EBA-4EF8-9FD6-87A7A2CD7C3E}" name="system_user_laboratory" displayName="system_user_laboratory" ref="I17:K23" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="I17:K23" xr:uid="{53A918CD-5EBA-4EF8-9FD6-87A7A2CD7C3E}"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{53A918CD-5EBA-4EF8-9FD6-87A7A2CD7C3E}" name="system_user_laboratory" displayName="system_user_laboratory" ref="I17:L23" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="I17:L23" xr:uid="{53A918CD-5EBA-4EF8-9FD6-87A7A2CD7C3E}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{A6876E42-44EF-4956-AF69-3C2D6B04F05D}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{7A325E24-BE39-48DA-9EE7-B0D3B27379C5}" uniqueName="2" name="user_id" queryTableFieldId="2" dataDxfId="39"/>
-    <tableColumn id="3" xr3:uid="{BE2AB8FB-6C0D-472C-B196-BA1BF6251146}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="38"/>
+    <tableColumn id="4" xr3:uid="{07997AD6-41DE-434E-B170-F78E25EFD917}" uniqueName="4" name="allowed" queryTableFieldId="4"/>
+    <tableColumn id="2" xr3:uid="{7A325E24-BE39-48DA-9EE7-B0D3B27379C5}" uniqueName="2" name="user_id" queryTableFieldId="2" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{BE2AB8FB-6C0D-472C-B196-BA1BF6251146}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1537,15 +1517,15 @@
   <autoFilter ref="M3:V10" xr:uid="{57C59DB0-9249-446E-B77D-DB2AD692BD9E}"/>
   <tableColumns count="10">
     <tableColumn id="1" xr3:uid="{CF9F54B0-2B16-4803-B797-3062E9C610A7}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{78188164-6FB0-4347-98E4-08F5EE17E7A6}" uniqueName="2" name="enviroment_id" queryTableFieldId="2" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{78188164-6FB0-4347-98E4-08F5EE17E7A6}" uniqueName="2" name="enviroment_id" queryTableFieldId="2" dataDxfId="34"/>
     <tableColumn id="3" xr3:uid="{504E1429-7582-48F2-9EFB-10FA5FC36F67}" uniqueName="3" name="qtd_computers" queryTableFieldId="3"/>
     <tableColumn id="4" xr3:uid="{A5BB4F58-0B79-4B51-AA4D-D9A122CAECBA}" uniqueName="4" name="qtd_chairs" queryTableFieldId="4"/>
     <tableColumn id="5" xr3:uid="{C91A198F-486D-4FF7-8134-3A0EC3966A55}" uniqueName="5" name="television" queryTableFieldId="5"/>
     <tableColumn id="6" xr3:uid="{385349E3-86B2-4907-8665-FC59A3BB2ABF}" uniqueName="6" name="fan" queryTableFieldId="6"/>
     <tableColumn id="7" xr3:uid="{821EC72B-DABC-4539-87B8-3A65E6E55C50}" uniqueName="7" name="air_conditioner" queryTableFieldId="7"/>
-    <tableColumn id="8" xr3:uid="{D38230E2-658A-495F-9DFE-3C9960243C45}" uniqueName="8" name="opening_time" queryTableFieldId="8" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{37E81A61-9516-4998-AF1E-4C302EBD35F1}" uniqueName="9" name="closing_time" queryTableFieldId="9" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{F34F4038-7D72-46D5-A4A6-38C4C9A0E11D}" uniqueName="10" name="is_activated" queryTableFieldId="10" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{D38230E2-658A-495F-9DFE-3C9960243C45}" uniqueName="8" name="opening_time" queryTableFieldId="8" dataDxfId="33"/>
+    <tableColumn id="9" xr3:uid="{37E81A61-9516-4998-AF1E-4C302EBD35F1}" uniqueName="9" name="closing_time" queryTableFieldId="9" dataDxfId="32"/>
+    <tableColumn id="10" xr3:uid="{F34F4038-7D72-46D5-A4A6-38C4C9A0E11D}" uniqueName="10" name="is_activated" queryTableFieldId="10" dataDxfId="31"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1557,13 +1537,13 @@
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{E8957FF5-5CF1-48BE-B563-9D045094127B}" uniqueName="1" name="id" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{1EA86638-7101-46C9-AE97-A79DB947852D}" uniqueName="2" name="registery" queryTableFieldId="2"/>
-    <tableColumn id="3" xr3:uid="{DAAA3AC6-32B6-4B92-848E-82BC6B6135B9}" uniqueName="3" name="type" queryTableFieldId="3" dataDxfId="34"/>
-    <tableColumn id="4" xr3:uid="{6F158A4B-EEB4-4EF1-AA68-EB005873D22D}" uniqueName="4" name="name" queryTableFieldId="4" dataDxfId="33"/>
-    <tableColumn id="5" xr3:uid="{EB6896FB-AF75-4511-9371-9B9F5D8DD646}" uniqueName="5" name="email" queryTableFieldId="5" dataDxfId="32"/>
-    <tableColumn id="6" xr3:uid="{882919FE-1CCF-46B5-9E1D-EFE6F9E221F0}" uniqueName="6" name="password" queryTableFieldId="6" dataDxfId="31"/>
-    <tableColumn id="7" xr3:uid="{F197965F-C0E5-4D0E-A0C8-38DCFD90D9AC}" uniqueName="7" name="entry_time" queryTableFieldId="7" dataDxfId="30"/>
-    <tableColumn id="8" xr3:uid="{BCD822DB-C994-4301-8B4B-AB18371426B6}" uniqueName="8" name="departure_time" queryTableFieldId="8" dataDxfId="29"/>
-    <tableColumn id="9" xr3:uid="{03BB6B96-6738-4D16-8BB1-5856A5FADCCB}" uniqueName="9" name="is_activated" queryTableFieldId="9" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{DAAA3AC6-32B6-4B92-848E-82BC6B6135B9}" uniqueName="3" name="type" queryTableFieldId="3" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{6F158A4B-EEB4-4EF1-AA68-EB005873D22D}" uniqueName="4" name="name" queryTableFieldId="4" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{EB6896FB-AF75-4511-9371-9B9F5D8DD646}" uniqueName="5" name="email" queryTableFieldId="5" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{882919FE-1CCF-46B5-9E1D-EFE6F9E221F0}" uniqueName="6" name="password" queryTableFieldId="6" dataDxfId="27"/>
+    <tableColumn id="7" xr3:uid="{F197965F-C0E5-4D0E-A0C8-38DCFD90D9AC}" uniqueName="7" name="entry_time" queryTableFieldId="7" dataDxfId="26"/>
+    <tableColumn id="8" xr3:uid="{BCD822DB-C994-4301-8B4B-AB18371426B6}" uniqueName="8" name="departure_time" queryTableFieldId="8" dataDxfId="25"/>
+    <tableColumn id="9" xr3:uid="{03BB6B96-6738-4D16-8BB1-5856A5FADCCB}" uniqueName="9" name="is_activated" queryTableFieldId="9" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1574,10 +1554,10 @@
   <autoFilter ref="B3:G20" xr:uid="{CCE5E823-FA9A-46C1-AEE5-A1F4D26E97D2}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{6DD82B72-16FA-4522-9E0D-76CD3A296400}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{DB60987B-C92B-4400-9315-A645299F690D}" uniqueName="2" name="type" queryTableFieldId="2" dataDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{155B98F5-19F9-4323-8010-D88AEC622683}" uniqueName="3" name="create_time" queryTableFieldId="3" dataDxfId="27"/>
-    <tableColumn id="4" xr3:uid="{5DD35A2A-535E-4AC9-AD6E-9C57089C59EA}" uniqueName="4" name="desc" queryTableFieldId="4" dataDxfId="26"/>
-    <tableColumn id="5" xr3:uid="{6799B699-560A-4E69-B293-35BFF90C76F4}" uniqueName="5" name="children_logs" queryTableFieldId="5" dataDxfId="25"/>
+    <tableColumn id="2" xr3:uid="{DB60987B-C92B-4400-9315-A645299F690D}" uniqueName="2" name="type" queryTableFieldId="2" dataDxfId="23"/>
+    <tableColumn id="3" xr3:uid="{155B98F5-19F9-4323-8010-D88AEC622683}" uniqueName="3" name="create_time" queryTableFieldId="3" dataDxfId="22"/>
+    <tableColumn id="4" xr3:uid="{5DD35A2A-535E-4AC9-AD6E-9C57089C59EA}" uniqueName="4" name="desc" queryTableFieldId="4" dataDxfId="21"/>
+    <tableColumn id="5" xr3:uid="{6799B699-560A-4E69-B293-35BFF90C76F4}" uniqueName="5" name="children_logs" queryTableFieldId="5" dataDxfId="20"/>
     <tableColumn id="6" xr3:uid="{C9D06D86-02D2-4AA9-B04D-10B8753863E4}" uniqueName="6" name="responsible_user" queryTableFieldId="6"/>
   </tableColumns>
   <tableStyleInfo name="generic" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1589,8 +1569,8 @@
   <autoFilter ref="B23:D26" xr:uid="{D29CA22D-8193-455B-B30F-40F9B9CD21C9}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{D8614071-7ED6-4F35-A407-2B26683179ED}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{5C87E7F9-259D-4C99-86D4-1187DB56973D}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="24"/>
-    <tableColumn id="3" xr3:uid="{22F785A3-4A76-4040-B33C-F9F005C7667B}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{5C87E7F9-259D-4C99-86D4-1187DB56973D}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="19"/>
+    <tableColumn id="3" xr3:uid="{22F785A3-4A76-4040-B33C-F9F005C7667B}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de Tabela 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1601,8 +1581,8 @@
   <autoFilter ref="F23:H26" xr:uid="{553991DF-4562-4DC9-B4D7-CACE9EC4EF9C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4110A2A1-680D-49EE-A555-BAB59838AABD}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{7C89E2E5-6182-4820-BB2D-018B26C39F30}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{5B1AA004-F95E-4671-98A9-F506460937ED}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{7C89E2E5-6182-4820-BB2D-018B26C39F30}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="17"/>
+    <tableColumn id="3" xr3:uid="{5B1AA004-F95E-4671-98A9-F506460937ED}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="16"/>
   </tableColumns>
   <tableStyleInfo name="Estilo de Tabela 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1613,23 +1593,22 @@
   <autoFilter ref="I3:L5" xr:uid="{2E646A49-017A-408A-9130-31769D85C05F}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{D3D491E2-3254-434B-A6D1-2BD498E19A2D}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{E42B4EE0-3A8F-47F8-A9FB-225337B26D45}" uniqueName="5" name="laboratory_list" queryTableFieldId="5" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{C3A4A2CF-8E80-435C-84B2-536EC81F67C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{10E92AEF-AA7D-4B7E-A6B2-9C4DFAD41D6F}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="18"/>
+    <tableColumn id="5" xr3:uid="{E42B4EE0-3A8F-47F8-A9FB-225337B26D45}" uniqueName="5" name="laboratory_list" queryTableFieldId="5" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{C3A4A2CF-8E80-435C-84B2-536EC81F67C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="14"/>
+    <tableColumn id="4" xr3:uid="{10E92AEF-AA7D-4B7E-A6B2-9C4DFAD41D6F}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{852D41C6-0DEC-4824-B44E-DEA0AE43A72A}" name="log_assosiation_user_laboratory" displayName="log_assosiation_user_laboratory" ref="I8:M13" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="I8:M13" xr:uid="{852D41C6-0DEC-4824-B44E-DEA0AE43A72A}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{852D41C6-0DEC-4824-B44E-DEA0AE43A72A}" name="log_assosiation_user_laboratory" displayName="log_assosiation_user_laboratory" ref="I8:L13" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="I8:L13" xr:uid="{852D41C6-0DEC-4824-B44E-DEA0AE43A72A}"/>
+  <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C910F50F-3F72-4039-8AE2-5D47546A804C}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="5" xr3:uid="{A042CA4C-1840-492F-9D9B-29679C65384A}" uniqueName="5" name="status" queryTableFieldId="5" dataDxfId="17"/>
-    <tableColumn id="2" xr3:uid="{3062A848-4CA3-4E74-B625-1F9A900401EC}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{09894099-35FD-4465-A043-0F0FA29B9B44}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="15"/>
-    <tableColumn id="4" xr3:uid="{2B76CF40-5649-4C92-840F-F3F52BA8BB01}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{3062A848-4CA3-4E74-B625-1F9A900401EC}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{09894099-35FD-4465-A043-0F0FA29B9B44}" uniqueName="3" name="laboratory_id" queryTableFieldId="3" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{2B76CF40-5649-4C92-840F-F3F52BA8BB01}" uniqueName="4" name="user_id" queryTableFieldId="4" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1640,10 +1619,10 @@
   <autoFilter ref="I16:M20" xr:uid="{FA7BCB58-3694-4DE3-9863-1776FE39B818}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{62BA4DE1-B2BB-4F72-BE20-471A357DC53B}" uniqueName="1" name="id" queryTableFieldId="1"/>
-    <tableColumn id="4" xr3:uid="{F1B0659D-A210-4A2D-B394-E87FB9BC2043}" uniqueName="4" name="operation_type" queryTableFieldId="4" dataDxfId="13"/>
-    <tableColumn id="5" xr3:uid="{FC65033A-F10C-4B71-852E-10A386498392}" uniqueName="5" name="session_key" queryTableFieldId="5" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{D4E4A59B-332D-44FC-80DC-6D187F5821C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{4619D07E-E77D-4FAC-9DD2-906F21BF18C8}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{F1B0659D-A210-4A2D-B394-E87FB9BC2043}" uniqueName="4" name="operation_type" queryTableFieldId="4" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{FC65033A-F10C-4B71-852E-10A386498392}" uniqueName="5" name="session_key" queryTableFieldId="5" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{D4E4A59B-332D-44FC-80DC-6D187F5821C4}" uniqueName="2" name="generic_id" queryTableFieldId="2" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{4619D07E-E77D-4FAC-9DD2-906F21BF18C8}" uniqueName="3" name="user_id" queryTableFieldId="3" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1969,7 +1948,7 @@
   <dimension ref="B2:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2046,7 +2025,7 @@
         <v>7</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="M3" t="s">
         <v>0</v>
@@ -2076,7 +2055,7 @@
         <v>49</v>
       </c>
       <c r="V3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:22" x14ac:dyDescent="0.25">
@@ -2104,7 +2083,7 @@
       <c r="I4" s="1">
         <v>0.75</v>
       </c>
-      <c r="J4" s="22" t="b">
+      <c r="J4" t="b">
         <v>1</v>
       </c>
       <c r="M4">
@@ -2163,7 +2142,7 @@
       <c r="I5" s="1">
         <v>0.72916666666666663</v>
       </c>
-      <c r="J5" s="22" t="b">
+      <c r="J5" t="b">
         <v>1</v>
       </c>
       <c r="M5">
@@ -2222,7 +2201,7 @@
       <c r="I6" s="1">
         <v>0.91666666666666663</v>
       </c>
-      <c r="J6" s="22" t="b">
+      <c r="J6" t="b">
         <v>0</v>
       </c>
       <c r="M6">
@@ -2281,7 +2260,7 @@
       <c r="I7" s="1">
         <v>0.51041666666666663</v>
       </c>
-      <c r="J7" s="22" t="b">
+      <c r="J7" t="b">
         <v>0</v>
       </c>
       <c r="M7">
@@ -2340,7 +2319,7 @@
       <c r="I8" s="1">
         <v>0.875</v>
       </c>
-      <c r="J8" s="22" t="b">
+      <c r="J8" t="b">
         <v>1</v>
       </c>
       <c r="M8">
@@ -2399,7 +2378,7 @@
       <c r="I9" s="1">
         <v>0.73958333333333337</v>
       </c>
-      <c r="J9" s="22" t="b">
+      <c r="J9" t="b">
         <v>1</v>
       </c>
       <c r="M9">
@@ -2458,7 +2437,7 @@
       <c r="I10" s="1">
         <v>0.9375</v>
       </c>
-      <c r="J10" s="22" t="b">
+      <c r="J10" t="b">
         <v>0</v>
       </c>
       <c r="M10">
@@ -2517,7 +2496,7 @@
       <c r="I11" s="1">
         <v>0.94444444444444442</v>
       </c>
-      <c r="J11" s="22" t="b">
+      <c r="J11" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2546,7 +2525,7 @@
       <c r="I12" s="1">
         <v>0.92708333333333337</v>
       </c>
-      <c r="J12" s="22" t="b">
+      <c r="J12" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2575,7 +2554,7 @@
       <c r="I13" s="1">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J13" s="22" t="b">
+      <c r="J13" t="b">
         <v>1</v>
       </c>
     </row>
@@ -2585,103 +2564,133 @@
       </c>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
-    </row>
-    <row r="17" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L16" s="13"/>
+    </row>
+    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I17" t="s">
         <v>0</v>
       </c>
-      <c r="J17" s="3" t="s">
+      <c r="J17" t="s">
+        <v>110</v>
+      </c>
+      <c r="K17" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="K17" s="4" t="s">
+      <c r="L17" s="4" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="18" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I18">
         <v>1</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" t="b">
+        <v>1</v>
+      </c>
+      <c r="K18" s="2">
         <v>2</v>
       </c>
-      <c r="K18" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="L18" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I19">
         <v>2</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" t="b">
+        <v>1</v>
+      </c>
+      <c r="K19" s="2">
         <v>3</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I20">
         <v>3</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" t="b">
+        <v>1</v>
+      </c>
+      <c r="K20" s="2">
         <v>5</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I21">
         <v>4</v>
       </c>
-      <c r="J21" s="2">
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" s="2">
         <v>6</v>
       </c>
-      <c r="K21" s="5">
+      <c r="L21" s="5">
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I22">
         <v>5</v>
       </c>
-      <c r="J22" s="2">
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" s="2">
         <v>9</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="9:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="9:12" x14ac:dyDescent="0.25">
       <c r="I23">
         <v>6</v>
       </c>
-      <c r="J23" s="2">
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" s="2">
         <v>10</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="I16:K16"/>
     <mergeCell ref="B2:J2"/>
     <mergeCell ref="M2:V2"/>
+    <mergeCell ref="I16:L16"/>
   </mergeCells>
   <conditionalFormatting sqref="J4:J13">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q4:V10">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>FALSE</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J18:J23">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2699,7 +2708,7 @@
   <dimension ref="B2:M26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2720,7 +2729,7 @@
   <sheetData>
     <row r="2" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B2" s="16" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C2" s="16"/>
       <c r="D2" s="16"/>
@@ -2728,7 +2737,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
       <c r="I2" s="19" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J2" s="19"/>
       <c r="K2" s="19"/>
@@ -2870,12 +2879,11 @@
         <v>1</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
       <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
     </row>
     <row r="8" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B8">
@@ -2899,16 +2907,13 @@
       <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="J8" t="s">
-        <v>96</v>
-      </c>
-      <c r="K8" s="7" t="s">
+      <c r="J8" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="M8" s="9" t="s">
+      <c r="L8" s="9" t="s">
         <v>57</v>
       </c>
     </row>
@@ -2934,16 +2939,13 @@
       <c r="I9">
         <v>1</v>
       </c>
-      <c r="J9" t="s">
-        <v>97</v>
-      </c>
-      <c r="K9" s="8">
+      <c r="J9" s="8">
         <v>10</v>
       </c>
-      <c r="L9" s="11">
-        <v>1</v>
-      </c>
-      <c r="M9" s="12">
+      <c r="K9" s="11">
+        <v>1</v>
+      </c>
+      <c r="L9" s="12">
         <v>2</v>
       </c>
     </row>
@@ -2969,16 +2971,13 @@
       <c r="I10">
         <v>2</v>
       </c>
-      <c r="J10" t="s">
-        <v>97</v>
-      </c>
-      <c r="K10" s="8">
+      <c r="J10" s="8">
         <v>11</v>
       </c>
-      <c r="L10" s="11">
+      <c r="K10" s="11">
         <v>3</v>
       </c>
-      <c r="M10" s="12">
+      <c r="L10" s="12">
         <v>3</v>
       </c>
     </row>
@@ -3004,16 +3003,13 @@
       <c r="I11">
         <v>3</v>
       </c>
-      <c r="J11" t="s">
-        <v>98</v>
-      </c>
-      <c r="K11" s="8">
+      <c r="J11" s="8">
         <v>12</v>
       </c>
-      <c r="L11" s="11">
-        <v>1</v>
-      </c>
-      <c r="M11" s="12">
+      <c r="K11" s="11">
+        <v>1</v>
+      </c>
+      <c r="L11" s="12">
         <v>2</v>
       </c>
     </row>
@@ -3039,16 +3035,13 @@
       <c r="I12">
         <v>4</v>
       </c>
-      <c r="J12" t="s">
-        <v>98</v>
-      </c>
-      <c r="K12" s="8">
+      <c r="J12" s="8">
         <v>16</v>
       </c>
-      <c r="L12" s="11">
+      <c r="K12" s="11">
         <v>4</v>
       </c>
-      <c r="M12" s="12">
+      <c r="L12" s="12">
         <v>10</v>
       </c>
     </row>
@@ -3074,16 +3067,13 @@
       <c r="I13">
         <v>5</v>
       </c>
-      <c r="J13" t="s">
-        <v>97</v>
-      </c>
-      <c r="K13" s="8">
+      <c r="J13" s="8">
         <v>17</v>
       </c>
-      <c r="L13" s="11">
-        <v>1</v>
-      </c>
-      <c r="M13" s="12">
+      <c r="K13" s="11">
+        <v>1</v>
+      </c>
+      <c r="L13" s="12">
         <v>10</v>
       </c>
     </row>
@@ -3127,7 +3117,7 @@
         <v>1</v>
       </c>
       <c r="I15" s="21" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="21"/>
@@ -3157,10 +3147,10 @@
         <v>0</v>
       </c>
       <c r="J16" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="K16" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="L16" s="7" t="s">
         <v>92</v>
@@ -3192,10 +3182,10 @@
         <v>1</v>
       </c>
       <c r="J17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K17" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L17" s="8">
         <v>7</v>
@@ -3227,10 +3217,10 @@
         <v>2</v>
       </c>
       <c r="J18" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K18" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="L18" s="8">
         <v>8</v>
@@ -3262,10 +3252,10 @@
         <v>3</v>
       </c>
       <c r="J19" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="K19" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="L19" s="8">
         <v>9</v>
@@ -3297,10 +3287,10 @@
         <v>4</v>
       </c>
       <c r="J20" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="K20" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="L20" s="8">
         <v>15</v>
@@ -3311,12 +3301,12 @@
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B22" s="17" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
       <c r="F22" s="18" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G22" s="18"/>
       <c r="H22" s="18"/>
@@ -3407,8 +3397,8 @@
     <mergeCell ref="B22:D22"/>
     <mergeCell ref="F22:H22"/>
     <mergeCell ref="I2:L2"/>
-    <mergeCell ref="I7:M7"/>
     <mergeCell ref="I15:M15"/>
+    <mergeCell ref="I7:L7"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <tableParts count="6">

</xml_diff>